<commit_message>
create Apache: CellService, ExcelService, SheetService move Book1 from test to main env create ExcelAspect, ExcelProperties remove ExcelTest add `spring-boot-starter-aop` dependency
</commit_message>
<xml_diff>
--- a/src/main/resources/static/Book1.xlsx
+++ b/src/main/resources/static/Book1.xlsx
@@ -14,6 +14,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet0" r:id="rId5" sheetId="2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
   <si>
     <t>22000</t>
   </si>
@@ -72,6 +73,18 @@
   </si>
   <si>
     <t>220000.0</t>
+  </si>
+  <si>
+    <t>1000.0</t>
+  </si>
+  <si>
+    <t>1asd</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>1asd23</t>
   </si>
 </sst>
 </file>
@@ -441,14 +454,14 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="n">
-        <v>1200000.0</v>
+        <v>123.0</v>
       </c>
       <c r="B1" s="1">
         <v>3225</v>
       </c>
       <c r="C1" t="n">
         <f>SUM(A:A)</f>
-        <v>1522685.7</v>
+        <v>322808.7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -534,4 +547,22 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>